<commit_message>
got the thing to work now
</commit_message>
<xml_diff>
--- a/EdurekaHybridFramework/src/conf/FacebookTestCases.xlsx
+++ b/EdurekaHybridFramework/src/conf/FacebookTestCases.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04B8EBB-0B8D-49C3-94EA-6A8FCE9FDDAE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B14CFF-E6B6-4C0E-B9E9-87157D3EE9B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="7710" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17235" windowHeight="7710" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="1" r:id="rId1"/>
-    <sheet name="BadPass" sheetId="12" r:id="rId2"/>
+    <sheet name="BadLogin" sheetId="12" r:id="rId2"/>
     <sheet name="NoFirstName" sheetId="18" r:id="rId3"/>
     <sheet name="NoLastName" sheetId="19" r:id="rId4"/>
     <sheet name="NoEmailAddrs" sheetId="20" r:id="rId5"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="78">
   <si>
     <t>click</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Runstatus</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -214,9 +211,6 @@
     <t>xpath:=//div[contains(text(), 'incorrect')]</t>
   </si>
   <si>
-    <t>BadPass</t>
-  </si>
-  <si>
     <t>NoFirstName</t>
   </si>
   <si>
@@ -254,6 +248,21 @@
   </si>
   <si>
     <t>name:=reg_passwd__</t>
+  </si>
+  <si>
+    <t>Edward</t>
+  </si>
+  <si>
+    <t>edmcd@yahoo</t>
+  </si>
+  <si>
+    <t>BadLogin</t>
+  </si>
+  <si>
+    <t>xpath:=//div[contains(text(),'valid mobile number')]</t>
+  </si>
+  <si>
+    <t>xpath:=//div[contains(text(),'use this when')]</t>
   </si>
 </sst>
 </file>
@@ -684,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,10 +728,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -732,10 +741,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -745,10 +754,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -758,10 +767,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -771,10 +780,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -818,7 +827,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -829,10 +838,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -843,7 +852,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -851,13 +860,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -868,10 +877,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -882,10 +891,10 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,7 +905,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,10 +913,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -917,6 +926,176 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41EF9AA6-8D01-4EA4-B374-2AE20F5422D1}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="39.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB80BB5-E29C-49A9-BCCE-6F0CA0156FB7}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -949,7 +1128,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -960,10 +1139,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,7 +1153,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -982,13 +1161,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -999,7 +1178,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1010,10 +1192,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1024,10 +1203,10 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1038,10 +1217,10 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1052,10 +1231,10 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1066,7 +1245,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1074,10 +1253,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1085,12 +1264,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BB80BB5-E29C-49A9-BCCE-6F0CA0156FB7}">
-  <dimension ref="A1:G8"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E83961-3DA3-4010-AF55-C4B416BD647E}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1119,7 +1298,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -1130,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1144,7 +1323,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1152,13 +1331,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1169,10 +1348,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1183,10 +1362,10 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1194,10 +1373,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1205,10 +1384,46 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1216,18 +1431,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E83961-3DA3-4010-AF55-C4B416BD647E}">
-  <dimension ref="A1:G8"/>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBE9C20-C612-4751-95DE-29E1CB551DC2}">
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="3" max="3" width="56.85546875" customWidth="1"/>
     <col min="4" max="4" width="39.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
@@ -1250,7 +1465,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>28</v>
@@ -1261,10 +1476,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1275,7 +1490,7 @@
         <v>4</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,13 +1498,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1300,10 +1515,10 @@
         <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D5" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1314,10 +1529,10 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1325,10 +1540,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1336,141 +1554,49 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDBE9C20-C612-4751-95DE-29E1CB551DC2}">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
+      <c r="C10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1553,12 +1679,12 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
@@ -1588,7 +1714,7 @@
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -1623,62 +1749,62 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>